<commit_message>
Add Pre 2017 data and compare pre to 2017
</commit_message>
<xml_diff>
--- a/LakePowellOutletModifications/LakePowellInterimMaximumFlows.xlsx
+++ b/LakePowellOutletModifications/LakePowellInterimMaximumFlows.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakePowellOutletModifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFAF89A-B94D-4325-95FA-1ACA5BAC5CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1067E55F-3FFA-413D-93BB-3620A5D61208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
@@ -142,7 +142,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -340,7 +340,7 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -685,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2A5F14-946D-4CB1-86E9-911200637E00}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -735,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AF7ACC-A075-4254-BA1A-C1D7DD8AEFC7}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1319,7 +1319,7 @@
     <col min="7" max="16384" width="8.7265625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="11" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>

</xml_diff>